<commit_message>
Update daily and intraday volume tables for Post-ZLB, Pre-ZLB, and ZLB to reflect the latest data changes
</commit_message>
<xml_diff>
--- a/output/table3/Table3_Post-ZLB_intraday_volume.xlsx
+++ b/output/table3/Table3_Post-ZLB_intraday_volume.xlsx
@@ -756,7 +756,7 @@
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="n">
-        <v>10.45769959207459</v>
+        <v>11.80724067599067</v>
       </c>
       <c r="AC3" t="inlineStr"/>
       <c r="AD3" t="inlineStr"/>
@@ -2524,7 +2524,7 @@
       <c r="Z27" t="inlineStr"/>
       <c r="AA27" t="inlineStr"/>
       <c r="AB27" t="n">
-        <v>28.82795214045213</v>
+        <v>198.3873472823473</v>
       </c>
       <c r="AC27" t="inlineStr"/>
       <c r="AD27" t="inlineStr"/>

</xml_diff>